<commit_message>
Working code and raw results
</commit_message>
<xml_diff>
--- a/Drag vs Velocity Friday Group.xlsx
+++ b/Drag vs Velocity Friday Group.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\MyCourses\MECH8135\lab5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Documents\GitHub\RocketHeight\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -132,7 +132,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.6834187955309718E-2"/>
+          <c:y val="2.4405596106243811E-2"/>
+          <c:w val="0.90769471249516931"/>
+          <c:h val="0.83549274291827946"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
@@ -178,8 +188,45 @@
             </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
+            <c:intercept val="0"/>
             <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.9140340656741899E-2"/>
+                  <c:y val="0.78331642904498477"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -287,11 +334,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="385230984"/>
-        <c:axId val="385231768"/>
+        <c:axId val="306797712"/>
+        <c:axId val="306802416"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="385230984"/>
+        <c:axId val="306797712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -404,12 +451,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385231768"/>
+        <c:crossAx val="306802416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="385231768"/>
+        <c:axId val="306802416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -522,7 +569,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385230984"/>
+        <c:crossAx val="306797712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1126,7 +1173,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="119" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1137,7 +1184,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8671560" cy="6294120"/>
+    <xdr:ext cx="8668550" cy="6291303"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>

</xml_diff>